<commit_message>
[EDIT] - verwoording stukje anal
</commit_message>
<xml_diff>
--- a/Documenten/BCLW_analise.xlsx
+++ b/Documenten/BCLW_analise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Dropbox\0_2_ICT_Academie\MBO\B.01 ANA Analyseren\Productie\01. Reader\20180101\Aanvullend\P8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delli\OneDrive\Documenten\RaspberryPi_bclw\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4DA312-B5AE-4AA9-9ADD-93D5BD881F23}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{EE4DA312-B5AE-4AA9-9ADD-93D5BD881F23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{086D5865-F863-4451-B139-470B4BF1F025}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="768" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="190">
   <si>
     <t>C1.0 Verwoorden.</t>
   </si>
@@ -2795,9 +2795,6 @@
     <t>C1.9 Modellen</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Het Functioneel ontwerp </t>
-  </si>
-  <si>
     <t>Fucties</t>
   </si>
   <si>
@@ -2822,9 +2819,6 @@
     <t>De uitwerking van het technisch ontwerp komt in nevenstaande tabbladen</t>
   </si>
   <si>
-    <t xml:space="preserve">2 Het Technisch ontwerp </t>
-  </si>
-  <si>
     <t>Datadictionairy</t>
   </si>
   <si>
@@ -2847,13 +2841,43 @@
   </si>
   <si>
     <t>Uitwerking Activiteiten diagram</t>
+  </si>
+  <si>
+    <t>beeld</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>bord herken model</t>
+  </si>
+  <si>
+    <t>lijn herken model</t>
+  </si>
+  <si>
+    <t>in frame 3 herkent het bord herken model 90% stopbord</t>
+  </si>
+  <si>
+    <t>in frame 4 herkent het bord herken model 82% voorangsbord</t>
+  </si>
+  <si>
+    <t>in frame 5 herkent het bord herken model 81% hert over de weg bord</t>
+  </si>
+  <si>
+    <t>in frame 1 herkent het lijn herken model 90% lijn geel</t>
+  </si>
+  <si>
+    <t>in frame 2 herkent het lijn herken model 85% lijn wit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="49">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3576,6 +3600,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3606,25 +3631,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3642,19 +3667,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3665,15 +3699,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3690,10 +3715,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4392,7 +4416,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4692,65 +4716,65 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" thickBot="1">
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+    <row r="4" spans="2:3">
+      <c r="B4" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="85"/>
-    </row>
-    <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+      <c r="C4" s="86"/>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="85"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="85" t="s">
+      <c r="C6" s="86"/>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="85"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="86"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" thickBot="1">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="85" t="s">
+    <row r="11" spans="2:3">
+      <c r="B11" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="86" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
+    <row r="12" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4773,9 +4797,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4822,74 +4846,74 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:19" ht="30.75" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="97" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:19" ht="44.25" customHeight="1">
+      <c r="A7" s="88"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-    </row>
-    <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="97" t="s">
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+    </row>
+    <row r="8" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A8" s="88"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="11" t="s">
         <v>45</v>
       </c>
@@ -4897,33 +4921,33 @@
       <c r="R10" s="13"/>
       <c r="S10" s="14"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="96"/>
-      <c r="S11" s="96"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="96"/>
-      <c r="S12" s="96"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
+      <c r="Q11" s="99"/>
+      <c r="R11" s="99"/>
+      <c r="S11" s="99"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="98"/>
+      <c r="Q12" s="99"/>
+      <c r="R12" s="99"/>
+      <c r="S12" s="99"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="98"/>
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="95"/>
-      <c r="R13" s="95"/>
-      <c r="S13" s="95"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q13" s="98"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="98"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="17" t="s">
         <v>48</v>
       </c>
@@ -4932,20 +4956,20 @@
       </c>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="M15" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="9"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
@@ -4959,22 +4983,22 @@
       <c r="R18" s="13"/>
       <c r="S18" s="14"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="96"/>
-      <c r="S19" s="96"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
+    <row r="19" spans="1:19">
+      <c r="A19" s="98"/>
+      <c r="Q19" s="99"/>
+      <c r="R19" s="99"/>
+      <c r="S19" s="99"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="98"/>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q20" s="99"/>
+      <c r="R20" s="99"/>
+      <c r="S20" s="99"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="17" t="s">
         <v>48</v>
       </c>
@@ -4984,22 +5008,17 @@
       <c r="C21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
-      <c r="S21" s="95"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A6:G8"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="H8:N8"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="Q20:S20"/>
@@ -5007,6 +5026,11 @@
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="Q12:S12"/>
     <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="A6:G8"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="H8:N8"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5018,9 +5042,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -5067,138 +5091,138 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+    <row r="6" spans="1:15" ht="27.75" customHeight="1">
+      <c r="A6" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="102" t="s">
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-    </row>
-    <row r="7" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="102" t="s">
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+    </row>
+    <row r="7" spans="1:15" ht="27" customHeight="1">
+      <c r="A7" s="105"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="103" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="107" t="s">
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="110" t="s">
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="111" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="111"/>
-    </row>
-    <row r="11" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="107" t="s">
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="112"/>
+    </row>
+    <row r="11" spans="1:15" ht="31.5" customHeight="1">
+      <c r="A11" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="102" t="s">
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-    </row>
-    <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="102" t="s">
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+    </row>
+    <row r="12" spans="1:15" ht="12.75" customHeight="1">
+      <c r="A12" s="105"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="103"/>
-    </row>
-    <row r="13" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="104"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="102" t="s">
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="104"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="104"/>
+    </row>
+    <row r="13" spans="1:15" ht="29.25" customHeight="1">
+      <c r="A13" s="105"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="103" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="103"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
-      <c r="N13" s="103"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="104"/>
+      <c r="N13" s="104"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="39" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="39"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -5209,12 +5233,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="B17" s="41" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>89</v>
       </c>
@@ -5225,7 +5249,7 @@
       <c r="G18" s="42"/>
       <c r="H18" s="30"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="C19" s="31"/>
       <c r="D19" s="43" t="s">
         <v>101</v>
@@ -5237,7 +5261,7 @@
       </c>
       <c r="H19" s="32"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="C20" s="33"/>
       <c r="D20" s="45"/>
       <c r="E20" s="34"/>
@@ -5245,7 +5269,7 @@
       <c r="G20" s="45"/>
       <c r="H20" s="34"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="C22" t="s">
         <v>46</v>
       </c>
@@ -5266,7 +5290,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="D23" s="46"/>
       <c r="E23" s="47"/>
       <c r="F23" s="41"/>
@@ -5274,7 +5298,7 @@
       <c r="H23" s="46"/>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="B24" s="48" t="s">
         <v>48</v>
       </c>
@@ -5289,7 +5313,7 @@
       </c>
       <c r="H24" s="51"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="C25" s="52"/>
       <c r="D25" s="53" t="s">
         <v>99</v>
@@ -5301,7 +5325,7 @@
       </c>
       <c r="H25" s="54"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
@@ -5309,25 +5333,25 @@
       <c r="G26" s="55"/>
       <c r="H26" s="55"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H11:N11"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="H12:N12"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="H13:N13"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5340,9 +5364,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -5389,136 +5413,136 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="62" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+    <row r="6" spans="1:15" ht="44.25" customHeight="1">
+      <c r="A6" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="18.75" customHeight="1">
+      <c r="A7" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
-    </row>
-    <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="107" t="s">
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+    </row>
+    <row r="9" spans="1:15" ht="30.75" customHeight="1">
+      <c r="A9" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="102" t="s">
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
-    </row>
-    <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+    </row>
+    <row r="10" spans="1:15" ht="30.75" customHeight="1">
+      <c r="A10" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="116"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="102" t="s">
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="103"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
-    </row>
-    <row r="11" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="104"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="102" t="s">
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
+    </row>
+    <row r="11" spans="1:15" ht="32.25" customHeight="1">
+      <c r="A11" s="105"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-    </row>
-    <row r="12" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="102" t="s">
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+    </row>
+    <row r="12" spans="1:15" ht="29.25" customHeight="1">
+      <c r="A12" s="105"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="103"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="104"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="104"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="B14" s="56" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="B16" s="56"/>
       <c r="D16" s="61" t="s">
         <v>114</v>
@@ -5527,7 +5551,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="B17" s="57" t="s">
         <v>91</v>
       </c>
@@ -5541,11 +5565,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="D18" s="31"/>
       <c r="G18" s="33"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" s="56" t="s">
         <v>92</v>
       </c>
@@ -5556,7 +5580,7 @@
       <c r="G19" s="42"/>
       <c r="H19" s="30"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="B20" s="56"/>
       <c r="C20" s="31"/>
       <c r="D20" s="44" t="s">
@@ -5569,7 +5593,7 @@
       </c>
       <c r="H20" s="32"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="B21" s="56"/>
       <c r="C21" s="33"/>
       <c r="D21" s="45"/>
@@ -5578,10 +5602,10 @@
       <c r="G21" s="45"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="B22" s="56"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="B23" s="56"/>
       <c r="C23" s="59" t="s">
         <v>94</v>
@@ -5599,7 +5623,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="B24" s="60" t="s">
         <v>48</v>
       </c>
@@ -5614,7 +5638,7 @@
       </c>
       <c r="H24" s="51"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="C25" s="49"/>
       <c r="D25" s="53" t="s">
         <v>99</v>
@@ -5626,25 +5650,25 @@
       </c>
       <c r="H25" s="51"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H11:N11"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="H12:N12"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5657,9 +5681,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -5706,37 +5730,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+    <row r="6" spans="1:15">
+      <c r="A6" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -5744,129 +5768,129 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="114" t="s">
+      <c r="H7" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="118" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="104"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="118" t="s">
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="105"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="120" t="s">
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="118" t="s">
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="104"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="118" t="s">
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="105"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="104"/>
-      <c r="B14" s="105"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="118" t="s">
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="105"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="118" t="s">
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="105"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17">
         <v>1</v>
       </c>
@@ -5874,18 +5898,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="C18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="C19" t="s">
         <v>69</v>
       </c>
       <c r="K19" s="25"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="B21">
         <v>2</v>
       </c>
@@ -5893,12 +5917,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="C22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="C23" t="s">
         <v>71</v>
       </c>
@@ -5906,15 +5930,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="28"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="28"/>
       <c r="C27" s="29" t="s">
         <v>74</v>
@@ -5925,7 +5949,7 @@
       </c>
       <c r="F27" s="30"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="28"/>
       <c r="C28" s="31"/>
       <c r="D28" s="32"/>
@@ -5936,7 +5960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="C29" s="33"/>
       <c r="D29" s="34"/>
       <c r="E29" s="33"/>
@@ -5944,7 +5968,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
       <c r="E30" s="37" t="s">
@@ -5954,7 +5978,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="C31" s="36"/>
       <c r="D31" s="36"/>
       <c r="E31" s="37" t="s">
@@ -5964,7 +5988,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
       <c r="E32" s="37" t="s">
@@ -5974,7 +5998,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="C33" s="36"/>
       <c r="D33" s="36"/>
       <c r="E33" s="37" t="s">
@@ -5984,7 +6008,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
       <c r="E34" s="38" t="s">
@@ -5994,7 +6018,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="38" t="s">
@@ -6004,7 +6028,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
       <c r="E36" s="37" t="s">
@@ -6014,7 +6038,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="C37" s="36"/>
       <c r="D37" s="36"/>
       <c r="E37" s="37" t="s">
@@ -6024,13 +6048,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="H10:N10"/>
+    <mergeCell ref="H7:N7"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="H15:N15"/>
     <mergeCell ref="A12:G12"/>
@@ -6039,13 +6070,6 @@
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="H14:N14"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="H7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6058,9 +6082,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6107,39 +6131,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+    <row r="6" spans="1:20">
+      <c r="A6" s="116" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
       <c r="Q6" s="66"/>
       <c r="S6" s="67"/>
     </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6147,42 +6171,42 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="114" t="s">
+      <c r="H7" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
       <c r="Q7" s="66"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="Q8" s="65"/>
       <c r="S8" s="68"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+    <row r="9" spans="1:20">
+      <c r="A9" s="116" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="118" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="119" t="s">
         <v>122</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-    </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6190,17 +6214,17 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="114" t="s">
+      <c r="H10" s="118" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-    </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+    </row>
+    <row r="11" spans="1:20" ht="15" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6208,35 +6232,35 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="118" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="118" t="s">
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="105"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="119" t="s">
         <v>126</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -6244,17 +6268,17 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="114" t="s">
+      <c r="H13" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -6262,17 +6286,17 @@
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="114" t="s">
+      <c r="H14" s="118" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -6280,18 +6304,18 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="114" t="s">
+      <c r="H15" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
       <c r="T15" s="69"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -6299,18 +6323,18 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="114" t="s">
+      <c r="H16" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="119"/>
-      <c r="J16" s="119"/>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
-      <c r="M16" s="119"/>
-      <c r="N16" s="119"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
       <c r="T16" s="68"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -6318,17 +6342,17 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="114" t="s">
+      <c r="H17" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119"/>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="119"/>
-      <c r="N17" s="119"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -6336,28 +6360,28 @@
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="114" t="s">
+      <c r="H18" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="119"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="119"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+    </row>
+    <row r="19" spans="1:20">
       <c r="T19" s="69"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="T20" s="68"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="B21" s="56" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="B23" s="56"/>
       <c r="D23" s="61" t="s">
         <v>114</v>
@@ -6366,7 +6390,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="B24" s="57" t="s">
         <v>91</v>
       </c>
@@ -6380,11 +6404,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="D25" s="31"/>
       <c r="G25" s="33"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="B26" s="56" t="s">
         <v>92</v>
       </c>
@@ -6395,7 +6419,7 @@
       <c r="G26" s="42"/>
       <c r="H26" s="30"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="B27" s="56"/>
       <c r="C27" s="31"/>
       <c r="D27" s="44" t="s">
@@ -6408,7 +6432,7 @@
       </c>
       <c r="H27" s="32"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="B28" s="56"/>
       <c r="C28" s="33"/>
       <c r="D28" s="45"/>
@@ -6417,10 +6441,10 @@
       <c r="G28" s="45"/>
       <c r="H28" s="70"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="B29" s="56"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="B30" s="56"/>
       <c r="C30" s="59" t="s">
         <v>94</v>
@@ -6438,7 +6462,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="B31" s="60" t="s">
         <v>48</v>
       </c>
@@ -6453,7 +6477,7 @@
       </c>
       <c r="H31" s="51"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="C32" s="49"/>
       <c r="D32" s="53" t="s">
         <v>99</v>
@@ -6465,7 +6489,7 @@
       </c>
       <c r="H32" s="51"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -6500,9 +6524,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6549,38 +6573,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+    <row r="6" spans="1:19">
+      <c r="A6" s="116" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
       <c r="Q6" s="66"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6588,18 +6612,18 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="114" t="s">
+      <c r="H7" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
       <c r="Q7" s="66"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -6607,18 +6631,18 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="114" t="s">
+      <c r="H8" s="118" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
       <c r="Q8" s="66"/>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -6626,18 +6650,18 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="114" t="s">
+      <c r="H9" s="118" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
       <c r="Q9" s="66"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6645,18 +6669,18 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="114" t="s">
+      <c r="H10" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
       <c r="Q10" s="66"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6664,18 +6688,18 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
       <c r="Q11" s="66"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -6683,18 +6707,18 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="114" t="s">
+      <c r="H12" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
       <c r="Q12" s="66"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -6702,18 +6726,18 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="114" t="s">
+      <c r="H13" s="118" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91"/>
       <c r="Q13" s="66"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -6721,18 +6745,18 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="114" t="s">
+      <c r="H14" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
       <c r="Q14" s="66"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -6740,34 +6764,34 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="114" t="s">
+      <c r="H15" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
       <c r="Q15" s="66"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="Q16" s="65"/>
       <c r="S16" s="68"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="T17" s="68"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="B18" s="56" t="s">
         <v>90</v>
       </c>
       <c r="T18" s="68"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="T19" s="68"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="B20" s="56"/>
       <c r="D20" s="61" t="s">
         <v>114</v>
@@ -6777,7 +6801,7 @@
       </c>
       <c r="T20" s="68"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="B21" s="57" t="s">
         <v>91</v>
       </c>
@@ -6792,12 +6816,12 @@
       </c>
       <c r="T21" s="68"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="D22" s="31"/>
       <c r="G22" s="33"/>
       <c r="T22" s="68"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="B23" s="56" t="s">
         <v>92</v>
       </c>
@@ -6809,7 +6833,7 @@
       <c r="H23" s="30"/>
       <c r="T23" s="68"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="B24" s="56"/>
       <c r="C24" s="31"/>
       <c r="D24" s="44" t="s">
@@ -6823,7 +6847,7 @@
       <c r="H24" s="32"/>
       <c r="T24" s="68"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="B25" s="56"/>
       <c r="C25" s="33"/>
       <c r="D25" s="45"/>
@@ -6833,11 +6857,11 @@
       <c r="H25" s="34"/>
       <c r="T25" s="68"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="B26" s="56"/>
       <c r="T26" s="68"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="B27" s="56"/>
       <c r="C27" s="59" t="s">
         <v>94</v>
@@ -6856,7 +6880,7 @@
       </c>
       <c r="T27" s="68"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="B28" s="60" t="s">
         <v>48</v>
       </c>
@@ -6872,7 +6896,7 @@
       <c r="H28" s="51"/>
       <c r="T28" s="68"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="C29" s="49"/>
       <c r="D29" s="53" t="s">
         <v>99</v>
@@ -6885,7 +6909,7 @@
       <c r="H29" s="51"/>
       <c r="T29" s="68"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -6915,9 +6939,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6964,41 +6988,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
+    <row r="6" spans="1:20">
+      <c r="A6" s="116" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
       <c r="Q6" s="66"/>
       <c r="R6" s="69"/>
       <c r="S6" s="68"/>
       <c r="T6" s="69"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -7006,21 +7030,21 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="114" t="s">
+      <c r="H7" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
       <c r="Q7" s="66"/>
       <c r="R7" s="69"/>
       <c r="S7" s="68"/>
       <c r="T7" s="69"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -7028,21 +7052,21 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="114" t="s">
+      <c r="H8" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
       <c r="Q8" s="66"/>
       <c r="R8" s="69"/>
       <c r="S8" s="68"/>
       <c r="T8" s="69"/>
     </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -7050,21 +7074,21 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="114" t="s">
+      <c r="H9" s="118" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
       <c r="Q9" s="66"/>
       <c r="R9" s="69"/>
       <c r="S9" s="68"/>
       <c r="T9" s="69"/>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -7072,21 +7096,21 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="114" t="s">
+      <c r="H10" s="118" t="s">
         <v>150</v>
       </c>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
       <c r="Q10" s="66"/>
       <c r="R10" s="69"/>
       <c r="S10" s="68"/>
       <c r="T10" s="69"/>
     </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -7094,19 +7118,19 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
       <c r="Q11" s="66"/>
       <c r="R11" s="69"/>
       <c r="S11" s="69"/>
       <c r="T11" s="69"/>
     </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -7114,19 +7138,19 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="114" t="s">
+      <c r="H12" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
       <c r="Q12" s="66"/>
       <c r="S12" s="69"/>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -7134,19 +7158,19 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="114" t="s">
+      <c r="H13" s="118" t="s">
         <v>152</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91"/>
       <c r="Q13" s="66"/>
       <c r="S13" s="69"/>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -7154,19 +7178,19 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="114" t="s">
+      <c r="H14" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
       <c r="Q14" s="66"/>
       <c r="S14" s="69"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -7174,34 +7198,34 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="114" t="s">
+      <c r="H15" s="118" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
       <c r="Q15" s="66"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="Q16" s="65"/>
       <c r="S16" s="68"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20">
       <c r="T17" s="68"/>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20">
       <c r="B18" s="56" t="s">
         <v>90</v>
       </c>
       <c r="T18" s="68"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20">
       <c r="T19" s="68"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20">
       <c r="B20" s="56"/>
       <c r="D20" s="61" t="s">
         <v>114</v>
@@ -7218,7 +7242,7 @@
       <c r="M20" s="54"/>
       <c r="T20" s="68"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20">
       <c r="B21" s="57" t="s">
         <v>91</v>
       </c>
@@ -7236,7 +7260,7 @@
       <c r="K21" s="41"/>
       <c r="T21" s="68"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20">
       <c r="D22" s="31"/>
       <c r="G22" s="33"/>
       <c r="I22" s="41"/>
@@ -7244,7 +7268,7 @@
       <c r="K22" s="41"/>
       <c r="T22" s="68"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20">
       <c r="B23" s="56" t="s">
         <v>92</v>
       </c>
@@ -7259,7 +7283,7 @@
       <c r="K23" s="76"/>
       <c r="T23" s="68"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20">
       <c r="B24" s="56"/>
       <c r="C24" s="31"/>
       <c r="D24" s="44" t="s">
@@ -7278,7 +7302,7 @@
       <c r="K24" s="77"/>
       <c r="T24" s="68"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20">
       <c r="B25" s="56"/>
       <c r="C25" s="33"/>
       <c r="D25" s="45"/>
@@ -7291,11 +7315,11 @@
       <c r="K25" s="79"/>
       <c r="T25" s="68"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20">
       <c r="B26" s="56"/>
       <c r="T26" s="68"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20">
       <c r="B27" s="56"/>
       <c r="C27" s="59" t="s">
         <v>94</v>
@@ -7314,7 +7338,7 @@
       </c>
       <c r="T27" s="68"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20">
       <c r="B28" s="56"/>
       <c r="C28" s="80" t="s">
         <v>155</v>
@@ -7326,7 +7350,7 @@
       <c r="H28" s="57"/>
       <c r="T28" s="68"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20">
       <c r="B29" s="60" t="s">
         <v>48</v>
       </c>
@@ -7342,7 +7366,7 @@
       <c r="H29" s="51"/>
       <c r="T29" s="68"/>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20">
       <c r="C30" s="49"/>
       <c r="D30" s="53" t="s">
         <v>99</v>
@@ -7355,24 +7379,24 @@
       <c r="H30" s="51"/>
       <c r="T30" s="68"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="H15:N15"/>
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="H8:N8"/>
     <mergeCell ref="H9:N9"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="H15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7385,9 +7409,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -7434,17 +7458,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="20" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="B8" s="81" t="s">
         <v>157</v>
       </c>
@@ -7452,7 +7476,7 @@
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75">
       <c r="B10" s="81" t="s">
         <v>158</v>
       </c>
@@ -7462,27 +7486,27 @@
       <c r="F10" s="41"/>
       <c r="G10" s="41"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="B12" s="82" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75">
       <c r="B14" s="83" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="C16" s="84" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="C19" s="84" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -7497,35 +7521,78 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="69" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="5" spans="2:3">
+      <c r="C5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>167</v>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7536,15 +7603,67 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED752DCA-8D76-432A-A777-3706FAB32113}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>169</v>
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7558,7 +7677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7566,15 +7685,67 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433504EA-A577-465B-995B-20D09D833E52}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>170</v>
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7584,15 +7755,67 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F21AE47-F189-47C6-8FE5-A7A33F4788D5}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>171</v>
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7605,40 +7828,81 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
+    <row r="1" spans="2:3" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="69" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="69" t="s">
+    <row r="5" spans="2:3">
+      <c r="C5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>177</v>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7648,15 +7912,67 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C3B3DC-0149-4091-977B-467E8D4C7316}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>178</v>
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7666,15 +7982,67 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422CF8E4-D259-41D0-A855-BB69C508F4ED}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
-        <v>179</v>
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7684,15 +8052,67 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295BE4D3-7693-4C88-8B7A-FDF2C0CE894E}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7702,15 +8122,67 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD99886-033D-4C2A-B732-1533D15336A3}">
-  <dimension ref="B1"/>
+  <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="123" t="s">
+    <row r="1" spans="2:2" ht="18.75">
+      <c r="B1" s="85" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7724,9 +8196,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1">
         <v>1</v>
       </c>
@@ -7782,38 +8254,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:18" ht="45.75" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -7833,9 +8305,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -7882,58 +8354,58 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="44.25" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="47.25" customHeight="1">
+      <c r="A7" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="89" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -7957,9 +8429,9 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8006,58 +8478,58 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="41.25" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="33.75" customHeight="1">
+      <c r="A7" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="89" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -8079,12 +8551,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="16" max="17" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8131,38 +8603,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="47.25" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -8182,9 +8654,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8231,66 +8703,66 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="36.75" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -8310,9 +8782,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8359,78 +8831,78 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="64.5" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="30.75" customHeight="1">
+      <c r="A7" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="89" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="8" spans="1:15" ht="33" customHeight="1">
+      <c r="A8" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="89" t="s">
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -8455,9 +8927,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8504,74 +8976,74 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:15" ht="57.75" customHeight="1">
+      <c r="A6" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+    </row>
+    <row r="7" spans="1:15" ht="42" customHeight="1">
+      <c r="A7" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="89" t="s">
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>51</v>
       </c>

</xml_diff>